<commit_message>
Added new testing data and updated the test report for PHA
</commit_message>
<xml_diff>
--- a/Test Excels/PHA_Crawler_Test_Excel.xlsx
+++ b/Test Excels/PHA_Crawler_Test_Excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D63C3E4-288C-485A-926A-596CEC798CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFC7A801-4F18-4566-8D32-38D086219AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
   <si>
     <t>pha_code</t>
   </si>
@@ -262,13 +262,145 @@
   </si>
   <si>
     <t>2025-10-15</t>
+  </si>
+  <si>
+    <t>PA008</t>
+  </si>
+  <si>
+    <t>Harrisburg Housing Authority</t>
+  </si>
+  <si>
+    <t>Harrisburg, PA</t>
+  </si>
+  <si>
+    <t>351 Chestnut St</t>
+  </si>
+  <si>
+    <t>Harrisburg</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Dauphin</t>
+  </si>
+  <si>
+    <t>Public Housing + HCV</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>https://www.harrisburghousing.org</t>
+  </si>
+  <si>
+    <t>&lt;scrape_date&gt;</t>
+  </si>
+  <si>
+    <t>&lt;version_hash&gt;</t>
+  </si>
+  <si>
+    <t>&lt;dataset_last_update&gt;</t>
+  </si>
+  <si>
+    <t>&lt;update_freq&gt;</t>
+  </si>
+  <si>
+    <t>&lt;data_license&gt;</t>
+  </si>
+  <si>
+    <t>&lt;crawler_run_data&gt;</t>
+  </si>
+  <si>
+    <t>717-232-6781</t>
+  </si>
+  <si>
+    <t>717-233-8355</t>
+  </si>
+  <si>
+    <t>hha@harrisburghousing.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2025-11-17</t>
+  </si>
+  <si>
+    <t>PA002</t>
+  </si>
+  <si>
+    <t>Philadelphia Housing Authority</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA</t>
+  </si>
+  <si>
+    <t>2013 Ridge Avenue</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>{single_parent":52%, "other":…}"</t>
+  </si>
+  <si>
+    <t>https://www.pha.phila.gov</t>
+  </si>
+  <si>
+    <t>215-684-4000</t>
+  </si>
+  <si>
+    <t>215-684-4163</t>
+  </si>
+  <si>
+    <t>info@pha.phila.gov</t>
+  </si>
+  <si>
+    <t>Kelvin A. Jeremiah</t>
+  </si>
+  <si>
+    <t>PA012</t>
+  </si>
+  <si>
+    <t>Montgomery County Housing Authority</t>
+  </si>
+  <si>
+    <t>Montgomery County, PA</t>
+  </si>
+  <si>
+    <t>2231 Hamilton Avenue / other offices</t>
+  </si>
+  <si>
+    <t>Willow Grove / Pottstown / Norristown</t>
+  </si>
+  <si>
+    <t>Montgomery</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>https://www.montcoha.org</t>
+  </si>
+  <si>
+    <t>610-275-5720</t>
+  </si>
+  <si>
+    <t>610-275-0889</t>
+  </si>
+  <si>
+    <t>joel.johnson@montcoha.org</t>
+  </si>
+  <si>
+    <t>Amanda Bone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +412,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -314,16 +454,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -624,13 +768,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:AU5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="14" max="14" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" customWidth="1"/>
+    <col min="26" max="26" width="18.7109375" customWidth="1"/>
+    <col min="27" max="27" width="17.28515625" customWidth="1"/>
+    <col min="28" max="28" width="22" customWidth="1"/>
+    <col min="29" max="29" width="23" customWidth="1"/>
+    <col min="30" max="30" width="21.7109375" customWidth="1"/>
+    <col min="31" max="31" width="24" customWidth="1"/>
+    <col min="32" max="32" width="20" customWidth="1"/>
+    <col min="33" max="33" width="24.140625" customWidth="1"/>
+    <col min="35" max="35" width="20.42578125" customWidth="1"/>
+    <col min="36" max="36" width="19.42578125" customWidth="1"/>
+    <col min="43" max="43" width="26.85546875" customWidth="1"/>
+    <col min="44" max="44" width="21.140625" customWidth="1"/>
+    <col min="45" max="45" width="18.5703125" customWidth="1"/>
+    <col min="46" max="46" width="20.140625" customWidth="1"/>
+    <col min="47" max="47" width="26.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
@@ -918,7 +1089,271 @@
         <v>76</v>
       </c>
     </row>
+    <row r="3" spans="1:47">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3">
+        <v>17101</v>
+      </c>
+      <c r="J3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3">
+        <v>1274</v>
+      </c>
+      <c r="N3">
+        <v>1640</v>
+      </c>
+      <c r="O3">
+        <v>2914</v>
+      </c>
+      <c r="S3">
+        <v>40.261899999999997</v>
+      </c>
+      <c r="T3">
+        <v>-76.881100000000004</v>
+      </c>
+      <c r="U3">
+        <v>25420</v>
+      </c>
+      <c r="V3" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y3">
+        <v>2025</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4">
+        <v>19121</v>
+      </c>
+      <c r="J4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4">
+        <v>18405</v>
+      </c>
+      <c r="N4">
+        <v>12972</v>
+      </c>
+      <c r="O4">
+        <v>31377</v>
+      </c>
+      <c r="S4">
+        <v>39.952599999999997</v>
+      </c>
+      <c r="T4">
+        <v>-75.165199999999999</v>
+      </c>
+      <c r="U4">
+        <v>37980</v>
+      </c>
+      <c r="V4" t="s">
+        <v>86</v>
+      </c>
+      <c r="W4">
+        <v>659730000</v>
+      </c>
+      <c r="Y4">
+        <v>2023</v>
+      </c>
+      <c r="Z4">
+        <v>20090.18</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5">
+        <v>19401</v>
+      </c>
+      <c r="J5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5">
+        <v>2260</v>
+      </c>
+      <c r="N5">
+        <v>550</v>
+      </c>
+      <c r="O5">
+        <v>2810</v>
+      </c>
+      <c r="Q5">
+        <v>0.95</v>
+      </c>
+      <c r="V5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU5" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AS5" r:id="rId1" xr:uid="{891B908D-6633-42A9-A543-DFFE21E99FB5}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the PHA javaFX report, added more attributes to be displayed
</commit_message>
<xml_diff>
--- a/Test Excels/PHA_Crawler_Test_Excel.xlsx
+++ b/Test Excels/PHA_Crawler_Test_Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFC7A801-4F18-4566-8D32-38D086219AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B93394A-E86D-46B1-9994-5BDBE976AEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="122">
   <si>
     <t>pha_code</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>hha@harrisburghousing.org</t>
+  </si>
+  <si>
+    <t>Senghor A. Manns</t>
   </si>
   <si>
     <t xml:space="preserve"> 2025-11-17</t>
@@ -770,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1174,25 +1177,28 @@
       <c r="AS3" t="s">
         <v>96</v>
       </c>
+      <c r="AT3" t="s">
+        <v>97</v>
+      </c>
       <c r="AU3" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:47">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
         <v>82</v>
@@ -1204,7 +1210,7 @@
         <v>19121</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L4" t="s">
         <v>85</v>
@@ -1240,10 +1246,10 @@
         <v>20090.18</v>
       </c>
       <c r="AB4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AL4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AM4" t="s">
         <v>88</v>
@@ -1258,36 +1264,36 @@
         <v>91</v>
       </c>
       <c r="AQ4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AR4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AS4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AT4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:47">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G5" t="s">
         <v>82</v>
@@ -1299,7 +1305,7 @@
         <v>19401</v>
       </c>
       <c r="J5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
         <v>85</v>
@@ -1317,10 +1323,10 @@
         <v>0.95</v>
       </c>
       <c r="V5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AL5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AM5" t="s">
         <v>88</v>
@@ -1335,19 +1341,19 @@
         <v>91</v>
       </c>
       <c r="AQ5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AR5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AS5" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AT5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AU5" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>